<commit_message>
Added bakery and washers tests
</commit_message>
<xml_diff>
--- a/pn-testing-framework/input-data/Test_FridgesSorting.xlsx
+++ b/pn-testing-framework/input-data/Test_FridgesSorting.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -25,10 +25,10 @@
     <t>название</t>
   </si>
   <si>
-    <t>Category</t>
+    <t>category</t>
   </si>
   <si>
-    <t>How to sort</t>
+    <t>howToSort</t>
   </si>
 </sst>
 </file>
@@ -80,7 +80,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -96,9 +96,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -136,9 +136,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -173,7 +173,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -208,7 +208,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -385,7 +385,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>